<commit_message>
added bobs wealth percent
</commit_message>
<xml_diff>
--- a/sp500 1916-2024 and Bobs money.xlsx
+++ b/sp500 1916-2024 and Bobs money.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aravn\Desktop\Courses\UIUC\CS416 - Data Visualization\Visual Narrative Project\CS416-Visual-Narrative-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58F2680-9C97-449F-9612-0AA8656D4CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3DB6FD-B828-42CA-AD0B-A6E47DD75EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9F420D7A-F405-4EB6-BA0E-C5D8B16B94B3}"/>
+    <workbookView xWindow="11235" yWindow="2670" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{9F420D7A-F405-4EB6-BA0E-C5D8B16B94B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="368">
   <si>
     <t>Date</t>
   </si>
@@ -1132,6 +1132,21 @@
   <si>
     <t>+10000</t>
   </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>bobs investments</t>
+  </si>
+  <si>
+    <t>bobs total investment</t>
+  </si>
+  <si>
+    <t>year end value</t>
+  </si>
+  <si>
+    <t>bobs year average</t>
+  </si>
 </sst>
 </file>
 
@@ -21217,6 +21232,503 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AE0916FE-238D-4EF8-941C-616FD3C81CC3}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="O5:P115" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="111">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="108"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item m="1" x="109"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="10" showAll="0"/>
+    <pivotField dataField="1" numFmtId="4" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="110">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="75"/>
+    </i>
+    <i>
+      <x v="76"/>
+    </i>
+    <i>
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="78"/>
+    </i>
+    <i>
+      <x v="79"/>
+    </i>
+    <i>
+      <x v="80"/>
+    </i>
+    <i>
+      <x v="81"/>
+    </i>
+    <i>
+      <x v="82"/>
+    </i>
+    <i>
+      <x v="83"/>
+    </i>
+    <i>
+      <x v="84"/>
+    </i>
+    <i>
+      <x v="85"/>
+    </i>
+    <i>
+      <x v="86"/>
+    </i>
+    <i>
+      <x v="87"/>
+    </i>
+    <i>
+      <x v="88"/>
+    </i>
+    <i>
+      <x v="89"/>
+    </i>
+    <i>
+      <x v="90"/>
+    </i>
+    <i>
+      <x v="91"/>
+    </i>
+    <i>
+      <x v="92"/>
+    </i>
+    <i>
+      <x v="93"/>
+    </i>
+    <i>
+      <x v="94"/>
+    </i>
+    <i>
+      <x v="95"/>
+    </i>
+    <i>
+      <x v="96"/>
+    </i>
+    <i>
+      <x v="97"/>
+    </i>
+    <i>
+      <x v="98"/>
+    </i>
+    <i>
+      <x v="99"/>
+    </i>
+    <i>
+      <x v="100"/>
+    </i>
+    <i>
+      <x v="101"/>
+    </i>
+    <i>
+      <x v="102"/>
+    </i>
+    <i>
+      <x v="103"/>
+    </i>
+    <i>
+      <x v="104"/>
+    </i>
+    <i>
+      <x v="105"/>
+    </i>
+    <i>
+      <x v="106"/>
+    </i>
+    <i>
+      <x v="107"/>
+    </i>
+    <i>
+      <x v="108"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of Amount ($)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -21537,8 +22049,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B1845"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A1596" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36346,7 +36858,7 @@
   <dimension ref="A1:G1845"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56835,10 +57347,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A72F4A-64F0-49E4-8B10-199AFAC16155}">
-  <dimension ref="A1:P1314"/>
+  <dimension ref="A1:R1314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K96" sqref="K96"/>
+    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56848,9 +57360,12 @@
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>355</v>
       </c>
@@ -56867,7 +57382,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1916</v>
       </c>
@@ -56883,8 +57398,14 @@
       <c r="E2">
         <v>10.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="H2" t="s">
+        <v>366</v>
+      </c>
+      <c r="O2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1916</v>
       </c>
@@ -56906,8 +57427,14 @@
       <c r="I3" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="O3" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="P3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1916</v>
       </c>
@@ -56924,7 +57451,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1916</v>
       </c>
@@ -56946,8 +57473,20 @@
       <c r="I5" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="J5" t="s">
+        <v>364</v>
+      </c>
+      <c r="K5" t="s">
+        <v>365</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="P5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1916</v>
       </c>
@@ -56969,12 +57508,23 @@
       <c r="I6">
         <v>0</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1916</v>
+      </c>
       <c r="P6">
-        <f>(5230.03-5000)/5000</f>
-        <v>4.600599999999995E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1916</v>
       </c>
@@ -56996,8 +57546,20 @@
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1917</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1916</v>
       </c>
@@ -57019,8 +57581,20 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1918</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1916</v>
       </c>
@@ -57042,8 +57616,20 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1919</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1916</v>
       </c>
@@ -57065,8 +57651,20 @@
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1920</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1916</v>
       </c>
@@ -57088,8 +57686,20 @@
       <c r="I11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1921</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1916</v>
       </c>
@@ -57111,8 +57721,20 @@
       <c r="I12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1922</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1916</v>
       </c>
@@ -57134,8 +57756,20 @@
       <c r="I13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1923</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1917</v>
       </c>
@@ -57157,8 +57791,20 @@
       <c r="I14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1924</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1917</v>
       </c>
@@ -57180,8 +57826,20 @@
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1925</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1917</v>
       </c>
@@ -57203,8 +57861,20 @@
       <c r="I16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1926</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>1917</v>
       </c>
@@ -57226,8 +57896,20 @@
       <c r="I17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1927</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>1917</v>
       </c>
@@ -57249,8 +57931,20 @@
       <c r="I18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>1928</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>1917</v>
       </c>
@@ -57273,10 +57967,25 @@
         <v>0</v>
       </c>
       <c r="J19" s="20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>250</v>
+      </c>
+      <c r="K19">
+        <v>250</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1929</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="20">
+        <v>250</v>
+      </c>
+      <c r="R19">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>1917</v>
       </c>
@@ -57298,8 +58007,17 @@
       <c r="I20">
         <v>193.19</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>250</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="R20">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>1917</v>
       </c>
@@ -57321,8 +58039,20 @@
       <c r="I21">
         <v>107.81</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>250</v>
+      </c>
+      <c r="O21" s="2">
+        <v>1930</v>
+      </c>
+      <c r="P21">
+        <v>241.93666666666672</v>
+      </c>
+      <c r="R21">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>1917</v>
       </c>
@@ -57344,8 +58074,20 @@
       <c r="I22">
         <v>101.54</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>250</v>
+      </c>
+      <c r="O22" s="2">
+        <v>1931</v>
+      </c>
+      <c r="P22">
+        <v>162.24749999999997</v>
+      </c>
+      <c r="R22">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>1917</v>
       </c>
@@ -57367,8 +58109,20 @@
       <c r="I23">
         <v>159.16</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>250</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1932</v>
+      </c>
+      <c r="P23">
+        <v>93.908333333333317</v>
+      </c>
+      <c r="R23">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>1917</v>
       </c>
@@ -57390,8 +58144,20 @@
       <c r="I24">
         <v>146.41</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>250</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1933</v>
+      </c>
+      <c r="P24">
+        <v>136.99</v>
+      </c>
+      <c r="R24">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25">
         <v>1917</v>
       </c>
@@ -57413,8 +58179,20 @@
       <c r="I25">
         <v>226.83</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>250</v>
+      </c>
+      <c r="O25" s="2">
+        <v>1934</v>
+      </c>
+      <c r="P25">
+        <v>150.47999999999999</v>
+      </c>
+      <c r="R25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26">
         <v>1918</v>
       </c>
@@ -57436,8 +58214,20 @@
       <c r="I26">
         <v>300.64999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>250</v>
+      </c>
+      <c r="O26" s="2">
+        <v>1935</v>
+      </c>
+      <c r="P26">
+        <v>178.11583333333331</v>
+      </c>
+      <c r="R26">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>1918</v>
       </c>
@@ -57459,8 +58249,20 @@
       <c r="I27">
         <v>204.12</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>250</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1936</v>
+      </c>
+      <c r="P27">
+        <v>265.44666666666666</v>
+      </c>
+      <c r="R27">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>1918</v>
       </c>
@@ -57482,8 +58284,20 @@
       <c r="I28">
         <v>239.84</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>250</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1937</v>
+      </c>
+      <c r="P28">
+        <v>260.53666666666669</v>
+      </c>
+      <c r="R28">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>1918</v>
       </c>
@@ -57505,8 +58319,20 @@
       <c r="I29">
         <v>246.99</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>250</v>
+      </c>
+      <c r="O29" s="2">
+        <v>1938</v>
+      </c>
+      <c r="P29">
+        <v>217.30333333333337</v>
+      </c>
+      <c r="R29">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30">
         <v>1918</v>
       </c>
@@ -57528,8 +58354,20 @@
       <c r="I30">
         <v>224.98</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>250</v>
+      </c>
+      <c r="O30" s="2">
+        <v>1939</v>
+      </c>
+      <c r="P30">
+        <v>236.875</v>
+      </c>
+      <c r="R30">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31">
         <v>1918</v>
       </c>
@@ -57551,8 +58389,20 @@
       <c r="I31">
         <v>204.52</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>250</v>
+      </c>
+      <c r="O31" s="2">
+        <v>1940</v>
+      </c>
+      <c r="P31">
+        <v>225.23249999999999</v>
+      </c>
+      <c r="R31">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32">
         <v>1918</v>
       </c>
@@ -57574,8 +58424,20 @@
       <c r="I32">
         <v>248.98</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="K32">
+        <v>250</v>
+      </c>
+      <c r="O32" s="2">
+        <v>1941</v>
+      </c>
+      <c r="P32">
+        <v>214.50333333333336</v>
+      </c>
+      <c r="R32">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33">
         <v>1918</v>
       </c>
@@ -57597,8 +58459,20 @@
       <c r="I33">
         <v>307.74</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="K33">
+        <v>250</v>
+      </c>
+      <c r="O33" s="2">
+        <v>1942</v>
+      </c>
+      <c r="P33">
+        <v>209.99749999999997</v>
+      </c>
+      <c r="R33">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34">
         <v>1918</v>
       </c>
@@ -57620,8 +58494,20 @@
       <c r="I34">
         <v>368.27</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="K34">
+        <v>250</v>
+      </c>
+      <c r="O34" s="2">
+        <v>1943</v>
+      </c>
+      <c r="P34">
+        <v>295.68</v>
+      </c>
+      <c r="R34">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35">
         <v>1918</v>
       </c>
@@ -57643,8 +58529,20 @@
       <c r="I35">
         <v>513.16</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="K35">
+        <v>250</v>
+      </c>
+      <c r="O35" s="2">
+        <v>1944</v>
+      </c>
+      <c r="P35">
+        <v>336.63666666666666</v>
+      </c>
+      <c r="R35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36">
         <v>1918</v>
       </c>
@@ -57666,8 +58564,20 @@
       <c r="I36">
         <v>451.31</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="K36">
+        <v>250</v>
+      </c>
+      <c r="O36" s="2">
+        <v>1945</v>
+      </c>
+      <c r="P36">
+        <v>434.70166666666665</v>
+      </c>
+      <c r="R36">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37">
         <v>1918</v>
       </c>
@@ -57689,8 +58599,20 @@
       <c r="I37">
         <v>462.87</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="K37">
+        <v>250</v>
+      </c>
+      <c r="O37" s="2">
+        <v>1946</v>
+      </c>
+      <c r="P37">
+        <v>489.53749999999997</v>
+      </c>
+      <c r="R37">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38">
         <v>1919</v>
       </c>
@@ -57712,8 +58634,20 @@
       <c r="I38">
         <v>506.87</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="K38">
+        <v>250</v>
+      </c>
+      <c r="O38" s="2">
+        <v>1947</v>
+      </c>
+      <c r="P38">
+        <v>461.21749999999992</v>
+      </c>
+      <c r="R38">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39">
         <v>1919</v>
       </c>
@@ -57735,8 +58669,20 @@
       <c r="I39">
         <v>595.49</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="K39">
+        <v>250</v>
+      </c>
+      <c r="O39" s="2">
+        <v>1948</v>
+      </c>
+      <c r="P39">
+        <v>501.13083333333333</v>
+      </c>
+      <c r="R39">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40">
         <v>1919</v>
       </c>
@@ -57758,8 +58704,20 @@
       <c r="I40">
         <v>800.23</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="K40">
+        <v>250</v>
+      </c>
+      <c r="O40" s="2">
+        <v>1949</v>
+      </c>
+      <c r="P40">
+        <v>525.91083333333336</v>
+      </c>
+      <c r="R40">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41">
         <v>1919</v>
       </c>
@@ -57781,8 +58739,20 @@
       <c r="I41">
         <v>975.61</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="K41">
+        <v>250</v>
+      </c>
+      <c r="O41" s="2">
+        <v>1950</v>
+      </c>
+      <c r="P41">
+        <v>686.95333333333326</v>
+      </c>
+      <c r="R41">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42">
         <v>1919</v>
       </c>
@@ -57804,8 +58774,20 @@
       <c r="I42">
         <v>1118.93</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="K42">
+        <v>250</v>
+      </c>
+      <c r="O42" s="2">
+        <v>1951</v>
+      </c>
+      <c r="P42">
+        <v>884.85250000000008</v>
+      </c>
+      <c r="R42">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43">
         <v>1919</v>
       </c>
@@ -57827,8 +58809,20 @@
       <c r="I43">
         <v>1152.5999999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="K43">
+        <v>250</v>
+      </c>
+      <c r="O43" s="2">
+        <v>1952</v>
+      </c>
+      <c r="P43">
+        <v>1027.5458333333333</v>
+      </c>
+      <c r="R43">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44">
         <v>1919</v>
       </c>
@@ -57850,8 +58844,20 @@
       <c r="I44">
         <v>1691.93</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="K44">
+        <v>250</v>
+      </c>
+      <c r="O44" s="2">
+        <v>1953</v>
+      </c>
+      <c r="P44">
+        <v>1087.4741666666669</v>
+      </c>
+      <c r="R44">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45">
         <v>1919</v>
       </c>
@@ -57873,8 +58879,20 @@
       <c r="I45">
         <v>2181.0500000000002</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="K45">
+        <v>250</v>
+      </c>
+      <c r="O45" s="2">
+        <v>1954</v>
+      </c>
+      <c r="P45">
+        <v>1422.9191666666668</v>
+      </c>
+      <c r="R45">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46">
         <v>1919</v>
       </c>
@@ -57896,8 +58914,20 @@
       <c r="I46">
         <v>2330.7800000000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="K46">
+        <v>250</v>
+      </c>
+      <c r="O46" s="2">
+        <v>1955</v>
+      </c>
+      <c r="P46">
+        <v>2002.7375</v>
+      </c>
+      <c r="R46">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47">
         <v>1919</v>
       </c>
@@ -57919,8 +58949,20 @@
       <c r="I47">
         <v>2195.37</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="K47">
+        <v>250</v>
+      </c>
+      <c r="O47" s="2">
+        <v>1956</v>
+      </c>
+      <c r="P47">
+        <v>2355.7741666666666</v>
+      </c>
+      <c r="R47">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48">
         <v>1919</v>
       </c>
@@ -57942,8 +58984,20 @@
       <c r="I48">
         <v>3081.96</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="K48">
+        <v>250</v>
+      </c>
+      <c r="O48" s="2">
+        <v>1957</v>
+      </c>
+      <c r="P48">
+        <v>2305.603333333333</v>
+      </c>
+      <c r="R48">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49">
         <v>1919</v>
       </c>
@@ -57965,8 +59019,20 @@
       <c r="I49">
         <v>3317.13</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="K49">
+        <v>250</v>
+      </c>
+      <c r="O49" s="2">
+        <v>1958</v>
+      </c>
+      <c r="P49">
+        <v>2590.3008333333332</v>
+      </c>
+      <c r="R49">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50">
         <v>1920</v>
       </c>
@@ -57988,8 +59054,20 @@
       <c r="I50">
         <v>3533.82</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="K50">
+        <v>250</v>
+      </c>
+      <c r="O50" s="2">
+        <v>1959</v>
+      </c>
+      <c r="P50">
+        <v>3245.24</v>
+      </c>
+      <c r="R50">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51">
         <v>1920</v>
       </c>
@@ -58011,8 +59089,20 @@
       <c r="I51">
         <v>4208.2700000000004</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="K51">
+        <v>250</v>
+      </c>
+      <c r="O51" s="2">
+        <v>1960</v>
+      </c>
+      <c r="P51">
+        <v>3261.5241666666666</v>
+      </c>
+      <c r="R51">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52">
         <v>1920</v>
       </c>
@@ -58034,8 +59124,20 @@
       <c r="I52">
         <v>4099.08</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="K52">
+        <v>250</v>
+      </c>
+      <c r="O52" s="2">
+        <v>1961</v>
+      </c>
+      <c r="P52">
+        <v>4033.1175000000003</v>
+      </c>
+      <c r="R52">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53">
         <v>1920</v>
       </c>
@@ -58057,8 +59159,20 @@
       <c r="I53">
         <v>4968.49</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="K53">
+        <v>250</v>
+      </c>
+      <c r="O53" s="2">
+        <v>1962</v>
+      </c>
+      <c r="P53">
+        <v>3846.5558333333338</v>
+      </c>
+      <c r="R53">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54">
         <v>1920</v>
       </c>
@@ -58080,8 +59194,20 @@
       <c r="I54">
         <v>5762.24</v>
       </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="K54">
+        <v>250</v>
+      </c>
+      <c r="O54" s="2">
+        <v>1963</v>
+      </c>
+      <c r="P54">
+        <v>4540.0058333333336</v>
+      </c>
+      <c r="R54">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
       <c r="A55">
         <v>1920</v>
       </c>
@@ -58103,8 +59229,20 @@
       <c r="I55">
         <v>6430.63</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="K55">
+        <v>250</v>
+      </c>
+      <c r="O55" s="2">
+        <v>1964</v>
+      </c>
+      <c r="P55">
+        <v>5427.1408333333329</v>
+      </c>
+      <c r="R55">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
       <c r="A56">
         <v>1920</v>
       </c>
@@ -58126,8 +59264,20 @@
       <c r="I56">
         <v>6018.12</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="K56">
+        <v>250</v>
+      </c>
+      <c r="O56" s="2">
+        <v>1965</v>
+      </c>
+      <c r="P56">
+        <v>6036.4158333333335</v>
+      </c>
+      <c r="R56">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
       <c r="A57">
         <v>1920</v>
       </c>
@@ -58149,8 +59299,20 @@
       <c r="I57">
         <v>6988.05</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="K57">
+        <v>250</v>
+      </c>
+      <c r="O57" s="2">
+        <v>1966</v>
+      </c>
+      <c r="P57">
+        <v>5925.2733333333335</v>
+      </c>
+      <c r="R57">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58">
         <v>1920</v>
       </c>
@@ -58172,8 +59334,20 @@
       <c r="I58">
         <v>7729.9</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="K58">
+        <v>250</v>
+      </c>
+      <c r="O58" s="2">
+        <v>1967</v>
+      </c>
+      <c r="P58">
+        <v>6729.8333333333348</v>
+      </c>
+      <c r="R58">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59">
         <v>1920</v>
       </c>
@@ -58195,8 +59369,20 @@
       <c r="I59">
         <v>7068.75</v>
       </c>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="K59">
+        <v>250</v>
+      </c>
+      <c r="O59" s="2">
+        <v>1968</v>
+      </c>
+      <c r="P59">
+        <v>7425.1258333333326</v>
+      </c>
+      <c r="R59">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60">
         <v>1920</v>
       </c>
@@ -58218,8 +59404,20 @@
       <c r="I60">
         <v>7601.99</v>
       </c>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="K60">
+        <v>250</v>
+      </c>
+      <c r="O60" s="2">
+        <v>1969</v>
+      </c>
+      <c r="P60">
+        <v>7465.100833333333</v>
+      </c>
+      <c r="R60">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61">
         <v>1920</v>
       </c>
@@ -58241,8 +59439,20 @@
       <c r="I61">
         <v>8666.2999999999993</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="K61">
+        <v>250</v>
+      </c>
+      <c r="O61" s="2">
+        <v>1970</v>
+      </c>
+      <c r="P61">
+        <v>6674.1150000000007</v>
+      </c>
+      <c r="R61">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62">
         <v>1921</v>
       </c>
@@ -58264,8 +59474,20 @@
       <c r="I62">
         <v>10214.459999999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="K62">
+        <v>250</v>
+      </c>
+      <c r="O62" s="2">
+        <v>1971</v>
+      </c>
+      <c r="P62">
+        <v>8195.9008333333331</v>
+      </c>
+      <c r="R62">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63">
         <v>1921</v>
       </c>
@@ -58287,8 +59509,20 @@
       <c r="I63">
         <v>8550.7000000000007</v>
       </c>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="K63">
+        <v>250</v>
+      </c>
+      <c r="O63" s="2">
+        <v>1972</v>
+      </c>
+      <c r="P63">
+        <v>9413.44</v>
+      </c>
+      <c r="R63">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64">
         <v>1921</v>
       </c>
@@ -58310,8 +59544,20 @@
       <c r="I64">
         <v>6748.62</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="K64">
+        <v>250</v>
+      </c>
+      <c r="O64" s="2">
+        <v>1973</v>
+      </c>
+      <c r="P64">
+        <v>9251.3383333333313</v>
+      </c>
+      <c r="R64">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65">
         <v>1921</v>
       </c>
@@ -58333,8 +59579,20 @@
       <c r="I65">
         <v>9393.4599999999991</v>
       </c>
-    </row>
-    <row r="66" spans="1:10">
+      <c r="K65">
+        <v>250</v>
+      </c>
+      <c r="O65" s="2">
+        <v>1974</v>
+      </c>
+      <c r="P65">
+        <v>7320.4508333333324</v>
+      </c>
+      <c r="R65">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66">
         <v>1921</v>
       </c>
@@ -58356,8 +59614,20 @@
       <c r="I66">
         <v>10446.4</v>
       </c>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="K66">
+        <v>250</v>
+      </c>
+      <c r="O66" s="2">
+        <v>1975</v>
+      </c>
+      <c r="P66">
+        <v>8395.8166666666657</v>
+      </c>
+      <c r="R66">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67">
         <v>1921</v>
       </c>
@@ -58379,8 +59649,20 @@
       <c r="I67">
         <v>9501.9699999999993</v>
       </c>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="K67">
+        <v>250</v>
+      </c>
+      <c r="O67" s="2">
+        <v>1976</v>
+      </c>
+      <c r="P67">
+        <v>10151.134166666665</v>
+      </c>
+      <c r="R67">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68">
         <v>1921</v>
       </c>
@@ -58402,8 +59684,20 @@
       <c r="I68">
         <v>11044.64</v>
       </c>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="K68">
+        <v>250</v>
+      </c>
+      <c r="O68" s="2">
+        <v>1977</v>
+      </c>
+      <c r="P68">
+        <v>9999.26</v>
+      </c>
+      <c r="R68">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69">
         <v>1921</v>
       </c>
@@ -58425,8 +59719,20 @@
       <c r="I69">
         <v>12934.97</v>
       </c>
-    </row>
-    <row r="70" spans="1:10">
+      <c r="K69">
+        <v>250</v>
+      </c>
+      <c r="O69" s="2">
+        <v>1978</v>
+      </c>
+      <c r="P69">
+        <v>10483.235833333332</v>
+      </c>
+      <c r="R69">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
       <c r="A70">
         <v>1921</v>
       </c>
@@ -58448,8 +59754,20 @@
       <c r="I70">
         <v>16300.67</v>
       </c>
-    </row>
-    <row r="71" spans="1:10">
+      <c r="K70">
+        <v>250</v>
+      </c>
+      <c r="O70" s="2">
+        <v>1979</v>
+      </c>
+      <c r="P70">
+        <v>11848.025</v>
+      </c>
+      <c r="R70">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71">
         <v>1921</v>
       </c>
@@ -58471,8 +59789,20 @@
       <c r="I71">
         <v>15123.62</v>
       </c>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="K71">
+        <v>250</v>
+      </c>
+      <c r="O71" s="2">
+        <v>1980</v>
+      </c>
+      <c r="P71">
+        <v>14482.772500000001</v>
+      </c>
+      <c r="R71">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72">
         <v>1921</v>
       </c>
@@ -58494,8 +59824,20 @@
       <c r="I72">
         <v>19677.91</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
+      <c r="K72">
+        <v>250</v>
+      </c>
+      <c r="O72" s="2">
+        <v>1981</v>
+      </c>
+      <c r="P72">
+        <v>15944.147500000001</v>
+      </c>
+      <c r="R72">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73">
         <v>1921</v>
       </c>
@@ -58517,8 +59859,20 @@
       <c r="I73">
         <v>23686.720000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="K73">
+        <v>250</v>
+      </c>
+      <c r="O73" s="2">
+        <v>1982</v>
+      </c>
+      <c r="P73">
+        <v>16253.695833333331</v>
+      </c>
+      <c r="R73">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74">
         <v>1922</v>
       </c>
@@ -58540,8 +59894,20 @@
       <c r="I74">
         <v>25561.67</v>
       </c>
-    </row>
-    <row r="75" spans="1:10">
+      <c r="K74">
+        <v>250</v>
+      </c>
+      <c r="O74" s="2">
+        <v>1983</v>
+      </c>
+      <c r="P74">
+        <v>22664.39</v>
+      </c>
+      <c r="R74">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
       <c r="A75">
         <v>1922</v>
       </c>
@@ -58563,8 +59929,20 @@
       <c r="I75">
         <v>32306.39</v>
       </c>
-    </row>
-    <row r="76" spans="1:10">
+      <c r="K75">
+        <v>250</v>
+      </c>
+      <c r="O75" s="2">
+        <v>1984</v>
+      </c>
+      <c r="P75">
+        <v>23488.115833333333</v>
+      </c>
+      <c r="R75">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
       <c r="A76">
         <v>1922</v>
       </c>
@@ -58586,8 +59964,20 @@
       <c r="I76">
         <v>42449.48</v>
       </c>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="K76">
+        <v>250</v>
+      </c>
+      <c r="O76" s="2">
+        <v>1985</v>
+      </c>
+      <c r="P76">
+        <v>28945.839166666672</v>
+      </c>
+      <c r="R76">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
       <c r="A77">
         <v>1922</v>
       </c>
@@ -58609,8 +59999,20 @@
       <c r="I77">
         <v>46314.14</v>
       </c>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="K77">
+        <v>250</v>
+      </c>
+      <c r="O77" s="2">
+        <v>1986</v>
+      </c>
+      <c r="P77">
+        <v>38114.373333333329</v>
+      </c>
+      <c r="R77">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
       <c r="A78">
         <v>1922</v>
       </c>
@@ -58635,8 +60037,20 @@
       <c r="J78" s="20" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="79" spans="1:10">
+      <c r="K78">
+        <v>5250</v>
+      </c>
+      <c r="O78" s="2">
+        <v>1987</v>
+      </c>
+      <c r="P78">
+        <v>52039.153333333328</v>
+      </c>
+      <c r="R78">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
       <c r="A79">
         <v>1922</v>
       </c>
@@ -58658,8 +60072,23 @@
       <c r="I79">
         <v>67160.89</v>
       </c>
-    </row>
-    <row r="80" spans="1:10">
+      <c r="K79">
+        <v>5250</v>
+      </c>
+      <c r="O79" s="2">
+        <v>1988</v>
+      </c>
+      <c r="P79">
+        <v>50625.003333333334</v>
+      </c>
+      <c r="Q79" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="R79">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
       <c r="A80">
         <v>1922</v>
       </c>
@@ -58681,8 +60110,20 @@
       <c r="I80">
         <v>66589.03</v>
       </c>
-    </row>
-    <row r="81" spans="1:10">
+      <c r="K80">
+        <v>5250</v>
+      </c>
+      <c r="O80" s="2">
+        <v>1989</v>
+      </c>
+      <c r="P80">
+        <v>63784.559166666673</v>
+      </c>
+      <c r="R80">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
       <c r="A81">
         <v>1922</v>
       </c>
@@ -58704,8 +60145,20 @@
       <c r="I81">
         <v>87865.71</v>
       </c>
-    </row>
-    <row r="82" spans="1:10">
+      <c r="K81">
+        <v>5250</v>
+      </c>
+      <c r="O81" s="2">
+        <v>1990</v>
+      </c>
+      <c r="P81">
+        <v>67070.952500000014</v>
+      </c>
+      <c r="R81">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
       <c r="A82">
         <v>1922</v>
       </c>
@@ -58727,8 +60180,20 @@
       <c r="I82">
         <v>94665.46</v>
       </c>
-    </row>
-    <row r="83" spans="1:10">
+      <c r="K82">
+        <v>5250</v>
+      </c>
+      <c r="O82" s="2">
+        <v>1991</v>
+      </c>
+      <c r="P82">
+        <v>79903.245833333334</v>
+      </c>
+      <c r="R82">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
       <c r="A83">
         <v>1922</v>
       </c>
@@ -58750,8 +60215,20 @@
       <c r="I83">
         <v>105746.64</v>
       </c>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="K83">
+        <v>5250</v>
+      </c>
+      <c r="O83" s="2">
+        <v>1992</v>
+      </c>
+      <c r="P83">
+        <v>89581.643333333355</v>
+      </c>
+      <c r="R83">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
       <c r="A84">
         <v>1922</v>
       </c>
@@ -58773,8 +60250,20 @@
       <c r="I84">
         <v>106965.2</v>
       </c>
-    </row>
-    <row r="85" spans="1:10">
+      <c r="K84">
+        <v>5250</v>
+      </c>
+      <c r="O84" s="2">
+        <v>1993</v>
+      </c>
+      <c r="P84">
+        <v>100384.35416666667</v>
+      </c>
+      <c r="R84">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
       <c r="A85">
         <v>1922</v>
       </c>
@@ -58796,8 +60285,20 @@
       <c r="I85">
         <v>144740.22</v>
       </c>
-    </row>
-    <row r="86" spans="1:10">
+      <c r="K85">
+        <v>5250</v>
+      </c>
+      <c r="O85" s="2">
+        <v>1994</v>
+      </c>
+      <c r="P85">
+        <v>104335.99166666665</v>
+      </c>
+      <c r="R85">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
       <c r="A86">
         <v>1923</v>
       </c>
@@ -58819,8 +60320,20 @@
       <c r="I86">
         <v>184345.89</v>
       </c>
-    </row>
-    <row r="87" spans="1:10">
+      <c r="K86">
+        <v>5250</v>
+      </c>
+      <c r="O86" s="2">
+        <v>1995</v>
+      </c>
+      <c r="P86">
+        <v>129205.74</v>
+      </c>
+      <c r="R86">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
       <c r="A87">
         <v>1923</v>
       </c>
@@ -58842,8 +60355,20 @@
       <c r="I87">
         <v>235796.2</v>
       </c>
-    </row>
-    <row r="88" spans="1:10">
+      <c r="K87">
+        <v>5250</v>
+      </c>
+      <c r="O87" s="2">
+        <v>1996</v>
+      </c>
+      <c r="P87">
+        <v>162941.89249999999</v>
+      </c>
+      <c r="R87">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
       <c r="A88">
         <v>1923</v>
       </c>
@@ -58865,8 +60390,20 @@
       <c r="I88">
         <v>310090.95</v>
       </c>
-    </row>
-    <row r="89" spans="1:10">
+      <c r="K88">
+        <v>5250</v>
+      </c>
+      <c r="O88" s="2">
+        <v>1997</v>
+      </c>
+      <c r="P88">
+        <v>216059.25166666671</v>
+      </c>
+      <c r="R88">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
       <c r="A89">
         <v>1923</v>
       </c>
@@ -58888,8 +60425,20 @@
       <c r="I89">
         <v>358389.82</v>
       </c>
-    </row>
-    <row r="90" spans="1:10">
+      <c r="K89">
+        <v>5250</v>
+      </c>
+      <c r="O89" s="2">
+        <v>1998</v>
+      </c>
+      <c r="P89">
+        <v>273404.86749999999</v>
+      </c>
+      <c r="R89">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
       <c r="A90">
         <v>1923</v>
       </c>
@@ -58911,8 +60460,20 @@
       <c r="I90">
         <v>349194.12</v>
       </c>
-    </row>
-    <row r="91" spans="1:10">
+      <c r="K90">
+        <v>5250</v>
+      </c>
+      <c r="O90" s="2">
+        <v>1999</v>
+      </c>
+      <c r="P90">
+        <v>335240.28833333327</v>
+      </c>
+      <c r="R90">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
       <c r="A91">
         <v>1923</v>
       </c>
@@ -58937,8 +60498,20 @@
       <c r="J91" s="20" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="92" spans="1:10">
+      <c r="K91">
+        <v>15250</v>
+      </c>
+      <c r="O91" s="2">
+        <v>2000</v>
+      </c>
+      <c r="P91">
+        <v>369111.20500000002</v>
+      </c>
+      <c r="R91">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18">
       <c r="A92">
         <v>1923</v>
       </c>
@@ -58960,8 +60533,23 @@
       <c r="I92">
         <v>241336.85</v>
       </c>
-    </row>
-    <row r="93" spans="1:10">
+      <c r="K92">
+        <v>15250</v>
+      </c>
+      <c r="O92" s="2">
+        <v>2001</v>
+      </c>
+      <c r="P92">
+        <v>309570.47999999992</v>
+      </c>
+      <c r="Q92" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="R92">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18">
       <c r="A93">
         <v>1923</v>
       </c>
@@ -58983,8 +60571,20 @@
       <c r="I93">
         <v>310284.12</v>
       </c>
-    </row>
-    <row r="94" spans="1:10">
+      <c r="K93">
+        <v>15250</v>
+      </c>
+      <c r="O93" s="2">
+        <v>2002</v>
+      </c>
+      <c r="P93">
+        <v>260530.83083333334</v>
+      </c>
+      <c r="R93">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18">
       <c r="A94">
         <v>1923</v>
       </c>
@@ -59006,8 +60606,20 @@
       <c r="I94">
         <v>329037.11</v>
       </c>
-    </row>
-    <row r="95" spans="1:10">
+      <c r="K94">
+        <v>15250</v>
+      </c>
+      <c r="O94" s="2">
+        <v>2003</v>
+      </c>
+      <c r="P94">
+        <v>267560.01583333331</v>
+      </c>
+      <c r="R94">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18">
       <c r="A95">
         <v>1923</v>
       </c>
@@ -59029,8 +60641,20 @@
       <c r="I95">
         <v>362339.41</v>
       </c>
-    </row>
-    <row r="96" spans="1:10">
+      <c r="K95">
+        <v>15250</v>
+      </c>
+      <c r="O95" s="2">
+        <v>2004</v>
+      </c>
+      <c r="P95">
+        <v>313636.10583333339</v>
+      </c>
+      <c r="R95">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18">
       <c r="A96">
         <v>1923</v>
       </c>
@@ -59052,8 +60676,20 @@
       <c r="I96">
         <v>410805.4</v>
       </c>
-    </row>
-    <row r="97" spans="1:10">
+      <c r="K96">
+        <v>15250</v>
+      </c>
+      <c r="O96" s="2">
+        <v>2005</v>
+      </c>
+      <c r="P96">
+        <v>341631.93583333329</v>
+      </c>
+      <c r="R96">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18">
       <c r="A97">
         <v>1923</v>
       </c>
@@ -59075,8 +60711,20 @@
       <c r="I97">
         <v>414748.29</v>
       </c>
-    </row>
-    <row r="98" spans="1:10">
+      <c r="K97">
+        <v>15250</v>
+      </c>
+      <c r="O97" s="2">
+        <v>2006</v>
+      </c>
+      <c r="P97">
+        <v>378539.65416666673</v>
+      </c>
+      <c r="R97">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18">
       <c r="A98">
         <v>1924</v>
       </c>
@@ -59101,8 +60749,20 @@
       <c r="J98" s="20" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="99" spans="1:10">
+      <c r="K98">
+        <v>25250</v>
+      </c>
+      <c r="O98" s="2">
+        <v>2007</v>
+      </c>
+      <c r="P98">
+        <v>439359.86166666658</v>
+      </c>
+      <c r="R98">
+        <v>15250</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18">
       <c r="A99">
         <v>1924</v>
       </c>
@@ -59124,8 +60784,23 @@
       <c r="I99">
         <v>355946.91</v>
       </c>
-    </row>
-    <row r="100" spans="1:10">
+      <c r="K99">
+        <v>25250</v>
+      </c>
+      <c r="O99" s="2">
+        <v>2008</v>
+      </c>
+      <c r="P99">
+        <v>358362.10166666663</v>
+      </c>
+      <c r="Q99" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="R99">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18">
       <c r="A100">
         <v>1924</v>
       </c>
@@ -59147,8 +60822,20 @@
       <c r="I100">
         <v>414257.09</v>
       </c>
-    </row>
-    <row r="101" spans="1:10">
+      <c r="K100">
+        <v>25250</v>
+      </c>
+      <c r="O100" s="2">
+        <v>2009</v>
+      </c>
+      <c r="P100">
+        <v>303731.45833333331</v>
+      </c>
+      <c r="R100">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18">
       <c r="A101">
         <v>1924</v>
       </c>
@@ -59170,8 +60857,20 @@
       <c r="I101">
         <v>428268.63</v>
       </c>
-    </row>
-    <row r="102" spans="1:10">
+      <c r="K101">
+        <v>25250</v>
+      </c>
+      <c r="O101" s="2">
+        <v>2010</v>
+      </c>
+      <c r="P101">
+        <v>369094.82833333331</v>
+      </c>
+      <c r="R101">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18">
       <c r="A102">
         <v>1924</v>
       </c>
@@ -59193,8 +60892,20 @@
       <c r="I102">
         <v>497617</v>
       </c>
-    </row>
-    <row r="103" spans="1:10">
+      <c r="K102">
+        <v>25250</v>
+      </c>
+      <c r="O102" s="2">
+        <v>2011</v>
+      </c>
+      <c r="P102">
+        <v>414422.60000000003</v>
+      </c>
+      <c r="R102">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18">
       <c r="A103">
         <v>1924</v>
       </c>
@@ -59216,8 +60927,20 @@
       <c r="I103">
         <v>624928.72</v>
       </c>
-    </row>
-    <row r="104" spans="1:10">
+      <c r="K103">
+        <v>25250</v>
+      </c>
+      <c r="O103" s="2">
+        <v>2012</v>
+      </c>
+      <c r="P103">
+        <v>464360.28499999997</v>
+      </c>
+      <c r="R103">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18">
       <c r="A104">
         <v>1924</v>
       </c>
@@ -59239,8 +60962,20 @@
       <c r="I104">
         <v>709026.27</v>
       </c>
-    </row>
-    <row r="105" spans="1:10">
+      <c r="K104">
+        <v>25250</v>
+      </c>
+      <c r="O104" s="2">
+        <v>2013</v>
+      </c>
+      <c r="P104">
+        <v>568066.18666666665</v>
+      </c>
+      <c r="R104">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18">
       <c r="A105">
         <v>1924</v>
       </c>
@@ -59262,8 +60997,20 @@
       <c r="I105">
         <v>684521.9</v>
       </c>
-    </row>
-    <row r="106" spans="1:10">
+      <c r="K105">
+        <v>25250</v>
+      </c>
+      <c r="O105" s="2">
+        <v>2014</v>
+      </c>
+      <c r="P105">
+        <v>675098.10749999993</v>
+      </c>
+      <c r="R105">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18">
       <c r="A106">
         <v>1924</v>
       </c>
@@ -59285,8 +61032,20 @@
       <c r="I106">
         <v>828967.03</v>
       </c>
-    </row>
-    <row r="107" spans="1:10">
+      <c r="K106">
+        <v>25250</v>
+      </c>
+      <c r="O106" s="2">
+        <v>2015</v>
+      </c>
+      <c r="P106">
+        <v>725084.51250000007</v>
+      </c>
+      <c r="R106">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18">
       <c r="A107">
         <v>1924</v>
       </c>
@@ -59308,8 +61067,20 @@
       <c r="I107">
         <v>1036043.38</v>
       </c>
-    </row>
-    <row r="108" spans="1:10">
+      <c r="K107">
+        <v>25250</v>
+      </c>
+      <c r="O107" s="2">
+        <v>2016</v>
+      </c>
+      <c r="P107">
+        <v>765934.0658333333</v>
+      </c>
+      <c r="R107">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18">
       <c r="A108">
         <v>1924</v>
       </c>
@@ -59331,8 +61102,20 @@
       <c r="I108">
         <v>986708.04</v>
       </c>
-    </row>
-    <row r="109" spans="1:10">
+      <c r="K108">
+        <v>25250</v>
+      </c>
+      <c r="O108" s="2">
+        <v>2017</v>
+      </c>
+      <c r="P108">
+        <v>917486.93500000006</v>
+      </c>
+      <c r="R108">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18">
       <c r="A109">
         <v>1924</v>
       </c>
@@ -59354,8 +61137,20 @@
       <c r="I109">
         <v>1264305.95</v>
       </c>
-    </row>
-    <row r="110" spans="1:10">
+      <c r="K109">
+        <v>25250</v>
+      </c>
+      <c r="O109" s="2">
+        <v>2018</v>
+      </c>
+      <c r="P109">
+        <v>1023843.8991666666</v>
+      </c>
+      <c r="R109">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18">
       <c r="A110">
         <v>1925</v>
       </c>
@@ -59377,8 +61172,20 @@
       <c r="I110">
         <v>1490189.44</v>
       </c>
-    </row>
-    <row r="111" spans="1:10">
+      <c r="K110">
+        <v>25250</v>
+      </c>
+      <c r="O110" s="2">
+        <v>2019</v>
+      </c>
+      <c r="P110">
+        <v>1135359.6216666666</v>
+      </c>
+      <c r="R110">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18">
       <c r="A111">
         <v>1925</v>
       </c>
@@ -59400,8 +61207,20 @@
       <c r="I111">
         <v>1821130.89</v>
       </c>
-    </row>
-    <row r="112" spans="1:10">
+      <c r="K111">
+        <v>25250</v>
+      </c>
+      <c r="O111" s="2">
+        <v>2020</v>
+      </c>
+      <c r="P111">
+        <v>1271628.6616666666</v>
+      </c>
+      <c r="R111">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18">
       <c r="A112">
         <v>1925</v>
       </c>
@@ -59426,8 +61245,20 @@
       <c r="J112" s="20" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="K112">
+        <v>35250</v>
+      </c>
+      <c r="O112" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P112">
+        <v>1714759.7066666668</v>
+      </c>
+      <c r="R112">
+        <v>25250</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18">
       <c r="A113">
         <v>1925</v>
       </c>
@@ -59449,8 +61280,23 @@
       <c r="I113">
         <v>1990033.22</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="K113">
+        <v>35250</v>
+      </c>
+      <c r="O113" s="2">
+        <v>2022</v>
+      </c>
+      <c r="P113">
+        <v>1634433.1283333332</v>
+      </c>
+      <c r="Q113" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="R113">
+        <v>35250</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18">
       <c r="A114">
         <v>1925</v>
       </c>
@@ -59472,8 +61318,17 @@
       <c r="I114">
         <v>184673.99185185184</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="O114" s="2">
+        <v>2023</v>
+      </c>
+      <c r="P114">
+        <v>1787585.7558333331</v>
+      </c>
+      <c r="R114">
+        <v>35250</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18">
       <c r="A115">
         <v>1925</v>
       </c>
@@ -59489,8 +61344,14 @@
       <c r="E115">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="O115" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="P115">
+        <v>174660.48907407399</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18">
       <c r="A116">
         <v>1925</v>
       </c>
@@ -59507,7 +61368,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:18">
       <c r="A117">
         <v>1925</v>
       </c>
@@ -59524,7 +61385,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:18">
       <c r="A118">
         <v>1925</v>
       </c>
@@ -59541,7 +61402,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:18">
       <c r="A119">
         <v>1925</v>
       </c>
@@ -59558,7 +61419,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:18">
       <c r="A120">
         <v>1925</v>
       </c>
@@ -59575,7 +61436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:18">
       <c r="A121">
         <v>1925</v>
       </c>
@@ -59592,7 +61453,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:18">
       <c r="A122">
         <v>1926</v>
       </c>
@@ -59609,7 +61470,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:18">
       <c r="A123">
         <v>1926</v>
       </c>
@@ -59626,7 +61487,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:18">
       <c r="A124">
         <v>1926</v>
       </c>
@@ -59643,7 +61504,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:18">
       <c r="A125">
         <v>1926</v>
       </c>
@@ -59660,7 +61521,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:18">
       <c r="A126">
         <v>1926</v>
       </c>
@@ -59677,7 +61538,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:18">
       <c r="A127">
         <v>1926</v>
       </c>
@@ -59694,7 +61555,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:18">
       <c r="A128">
         <v>1926</v>
       </c>

</xml_diff>